<commit_message>
Update on 16th Oct
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\Eclispse\SeleniumPractice\DataDrivenFrameworkMVN\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEBB81D-1C63-4A15-9071-91A516598C37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5650" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SoapUI" sheetId="10" r:id="rId1"/>
@@ -18,14 +19,18 @@
     <sheet name="PBLogin" sheetId="13" r:id="rId4"/>
     <sheet name="Quote" sheetId="6" r:id="rId5"/>
     <sheet name="Payment" sheetId="7" r:id="rId6"/>
-    <sheet name="Invoice" sheetId="3" r:id="rId7"/>
-    <sheet name="Term" sheetId="11" r:id="rId8"/>
-    <sheet name="dbTest" sheetId="9" r:id="rId9"/>
-    <sheet name="Delinquency" sheetId="12" r:id="rId10"/>
-    <sheet name="NSF" sheetId="4" r:id="rId11"/>
-    <sheet name="loginTest" sheetId="2" r:id="rId12"/>
-    <sheet name="process820Validation" sheetId="15" r:id="rId13"/>
-    <sheet name="Soap820" sheetId="16" r:id="rId14"/>
+    <sheet name="EDI834" sheetId="19" r:id="rId7"/>
+    <sheet name="Invoice" sheetId="3" r:id="rId8"/>
+    <sheet name="Term" sheetId="11" r:id="rId9"/>
+    <sheet name="FMSADMLogin" sheetId="18" r:id="rId10"/>
+    <sheet name="FMSADMINPWDRESET" sheetId="17" r:id="rId11"/>
+    <sheet name="dbTest" sheetId="9" r:id="rId12"/>
+    <sheet name="Delinquency" sheetId="12" r:id="rId13"/>
+    <sheet name="NSF" sheetId="4" r:id="rId14"/>
+    <sheet name="loginTest" sheetId="2" r:id="rId15"/>
+    <sheet name="process820Validation" sheetId="15" r:id="rId16"/>
+    <sheet name="Soap820" sheetId="16" r:id="rId17"/>
+    <sheet name="PaymentPortal" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>email</t>
   </si>
@@ -69,9 +74,6 @@
     <t>postMonth</t>
   </si>
   <si>
-    <t>08/2018</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -96,9 +98,6 @@
     <t>Delinquency</t>
   </si>
   <si>
-    <t>02/2019</t>
-  </si>
-  <si>
     <t>-100</t>
   </si>
   <si>
@@ -114,29 +113,80 @@
     <t>820Test</t>
   </si>
   <si>
-    <t>626916681011-H</t>
-  </si>
-  <si>
     <t>42690</t>
   </si>
   <si>
-    <t>09/30/2018</t>
-  </si>
-  <si>
-    <t>TC22SUB</t>
-  </si>
-  <si>
-    <t>626916681090-H</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>626916681121-H</t>
+  </si>
+  <si>
+    <t>626916681135-H</t>
+  </si>
+  <si>
+    <t>626916681136-D</t>
+  </si>
+  <si>
+    <t>04/2019</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confPassword</t>
+  </si>
+  <si>
+    <t>Password999</t>
+  </si>
+  <si>
+    <t>ccac0np3rf2</t>
+  </si>
+  <si>
+    <t>testper5</t>
+  </si>
+  <si>
+    <t>CarrierName</t>
+  </si>
+  <si>
+    <t>Bcbsma</t>
+  </si>
+  <si>
+    <t>717072019002-H</t>
+  </si>
+  <si>
+    <t>09/2019</t>
+  </si>
+  <si>
+    <t>b0ma8c0nsit2$</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>01/2019</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>700019091801-H</t>
+  </si>
+  <si>
+    <t>700019091802-H</t>
+  </si>
+  <si>
+    <t>12/31/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +202,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,17 +231,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,97 +572,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F568B8F9-86EC-4C18-8A89-BBA094E96B23}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3891170A-2B1F-44EB-815A-E460F81D59E5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -592,27 +718,117 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="Anuj11.Singh@nttdata.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E17:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Anuj11.Singh@nttdata.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="Anuj11.Singh@nttdata.com" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -643,18 +859,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,25 +884,25 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -697,12 +913,40 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519837E7-6D53-4E86-B188-42F40BF9E201}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -711,16 +955,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="13.26953125" customWidth="1"/>
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -733,26 +978,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -768,20 +1013,26 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -813,11 +1064,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,10 +1087,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -849,19 +1108,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
     <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -872,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -886,16 +1146,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -905,23 +1165,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A81409-6990-4294-8A1D-71EE5C71A5FF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -929,115 +1186,103 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D7A8DFDC-97D8-49A3-88A4-DCBA32B2515B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Anuj11.Singh@nttdata.com"/>
-  </hyperlinks>
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>